<commit_message>
[MOD] requeriments: se agrego la version del xlsx en la cual funciona el autofix
</commit_message>
<xml_diff>
--- a/custom/student_inscription/i18n/session_report.xlsx
+++ b/custom/student_inscription/i18n/session_report.xlsx
@@ -14,15 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
-  <si>
-    <t>My Company</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+  <si>
+    <t>UNEXCA</t>
   </si>
   <si>
     <t>Facultad</t>
   </si>
   <si>
-    <t>Rafael Daza</t>
+    <t>DCYT ciencias</t>
   </si>
   <si>
     <t>Curso</t>
@@ -34,25 +34,25 @@
     <t>Asunto</t>
   </si>
   <si>
-    <t>Calculo1</t>
+    <t>Programacion</t>
   </si>
   <si>
     <t>Hora de comienzo</t>
   </si>
   <si>
-    <t>11:38</t>
+    <t>00:41</t>
   </si>
   <si>
     <t>Dia</t>
   </si>
   <si>
-    <t>Thursday</t>
+    <t>Wednesday</t>
   </si>
   <si>
     <t>Unidades de Credito</t>
   </si>
   <si>
-    <t>4</t>
+    <t>2</t>
   </si>
   <si>
     <t>Tiempo</t>
@@ -70,7 +70,7 @@
     <t>Salon</t>
   </si>
   <si>
-    <t>L202</t>
+    <t>L-201</t>
   </si>
   <si>
     <t>Finaliza</t>
@@ -79,13 +79,13 @@
     <t>Sede</t>
   </si>
   <si>
-    <t>FLR</t>
+    <t>ALT</t>
   </si>
   <si>
     <t>Estudiantes:</t>
   </si>
   <si>
-    <t>2</t>
+    <t>1</t>
   </si>
   <si>
     <t>C.I.</t>
@@ -98,12 +98,6 @@
   </si>
   <si>
     <t>Mary Perez</t>
-  </si>
-  <si>
-    <t>4123123213</t>
-  </si>
-  <si>
-    <t>Andrea Lobo</t>
   </si>
 </sst>
 </file>
@@ -178,10 +172,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>4445</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>149860</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -199,7 +193,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3048000" y="190500"/>
-          <a:ext cx="857250" cy="228600"/>
+          <a:ext cx="1861820" cy="1102360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -212,8 +206,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B16:C18" totalsRowShown="0">
-  <autoFilter ref="B16:C18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B16:C17" totalsRowShown="0">
+  <autoFilter ref="B16:C17"/>
   <tableColumns count="2">
     <tableColumn id="1" name="C.I."/>
     <tableColumn id="2" name="Nombre del Estudiante"/>
@@ -507,11 +501,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:H18"/>
+  <dimension ref="B2:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:8">
       <c r="B2" s="1" t="s">
@@ -619,14 +620,6 @@
       </c>
       <c r="C17" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3">
-      <c r="B18" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>